<commit_message>
drop code? insert myself lib
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -485,7 +485,7 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>26/04/2025 01:40</t>
+          <t>27/04/2025 20:29</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
@@ -510,7 +510,7 @@
 Так же наши флористы могут собрать букет любой сложности, в любом
 оформлении - просто сообщите о своих пожеланиях при заказе менеджеру, и МЫ
 СДЕЛАЕМ КРАСИВО!
-Артикул позиции - ARTICLE572711
+Артикул позиции - ARTICLE505211
 Возможно, Вы искали: свежие цветы оптом, свежие тюльпаны, желтые, красные,
 розовые, фиолетовые
 ☎️</t>
@@ -523,7 +523,7 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>https://million-wallpapers.ru/wallpapers/4/29/17890145053225269085/nezhnyj-zh-ltyj-buket-roz.jpg https://million-wallpapers.ru/wallpapers/2/77/284157123227070/bukety-roz-alogo-krasnogo-i-belogo-cveta.jpg https://million-wallpapers.ru/wallpapers/0/4/10036622643701608943/krasivyj-buket-roz-v-vaze.jpg</t>
+          <t>https://million-wallpapers.ru//wallpapers/4/29/17890145053225269085/nezhnyj-zh-ltyj-buket-roz.jpg https://million-wallpapers.ru//wallpapers/2/77/284157123227070/bukety-roz-alogo-krasnogo-i-belogo-cveta.jpg</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -555,7 +555,7 @@
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>26/04/2025 01:40</t>
+          <t>27/04/2025 20:29</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
@@ -580,7 +580,7 @@
 Так же наши флористы могут собрать букет любой сложности, в любом
 оформлении - просто сообщите о своих пожеланиях при заказе менеджеру, и МЫ
 СДЕЛАЕМ КРАСИВО!
-Артикул позиции - ARTICLE833740
+Артикул позиции - ARTICLE629294
 Возможно, Вы искали: свежие цветы оптом, свежие тюльпаны, желтые, красные,
 розовые, фиолетовые
 ☎️</t>
@@ -593,7 +593,7 @@
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>https://million-wallpapers.ru/wallpapers/2/56/16878802474963253133/yarkij-i-svezhij-buket-romashek.jpg https://million-wallpapers.ru/wallpapers/4/62/15374319527758747808/nezhnaya-roza-v-bukete-dlya-devushki.jpg https://million-wallpapers.ru/wallpapers/5/80/362559507474470/krasnaya-roza-v-bukete-cvetov.jpg</t>
+          <t>https://million-wallpapers.ru//wallpapers/2/56/16878802474963253133/yarkij-i-svezhij-buket-romashek.jpg https://million-wallpapers.ru//wallpapers/4/62/15374319527758747808/nezhnaya-roza-v-bukete-dlya-devushki.jpg</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
@@ -625,7 +625,7 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>26/04/2025 01:40</t>
+          <t>27/04/2025 20:29</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
@@ -650,7 +650,7 @@
 Так же наши флористы могут собрать букет любой сложности, в любом
 оформлении - просто сообщите о своих пожеланиях при заказе менеджеру, и МЫ
 СДЕЛАЕМ КРАСИВО!
-Артикул позиции - ARTICLE241908
+Артикул позиции - ARTICLE522383
 Возможно, Вы искали: свежие цветы оптом, свежие тюльпаны, желтые, красные,
 розовые, фиолетовые
 ☎️</t>
@@ -663,7 +663,7 @@
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>https://million-wallpapers.ru/wallpapers/4/29/17890145053225269085/nezhnyj-zh-ltyj-buket-roz.jpg https://million-wallpapers.ru/wallpapers/2/77/284157123227070/bukety-roz-alogo-krasnogo-i-belogo-cveta.jpg https://million-wallpapers.ru/wallpapers/0/4/10036622643701608943/krasivyj-buket-roz-v-vaze.jpg</t>
+          <t>https://million-wallpapers.ru//wallpapers/4/29/17890145053225269085/nezhnyj-zh-ltyj-buket-roz.jpg https://million-wallpapers.ru//wallpapers/2/77/284157123227070/bukety-roz-alogo-krasnogo-i-belogo-cveta.jpg</t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
@@ -695,7 +695,7 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>26/04/2025 01:40</t>
+          <t>27/04/2025 20:29</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
@@ -720,7 +720,7 @@
 Так же наши флористы могут собрать букет любой сложности, в любом
 оформлении - просто сообщите о своих пожеланиях при заказе менеджеру, и МЫ
 СДЕЛАЕМ КРАСИВО!
-Артикул позиции - ARTICLE701934
+Артикул позиции - ARTICLE790651
 Возможно, Вы искали: свежие цветы оптом, свежие тюльпаны, желтые, красные,
 розовые, фиолетовые
 ☎️</t>
@@ -733,7 +733,7 @@
       </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>https://million-wallpapers.ru/wallpapers/5/82/456004843638851/buket-nezhnyx-rozovyx-roz.jpg https://million-wallpapers.ru/wallpapers/4/79/13477515223342528157/buket-iz-allyx-roz-vmvaze.jpg https://million-wallpapers.ru/wallpapers/4/41/15509849492199153317/buket-krasivyx-roza-cvetochnom-ryadu.jpg</t>
+          <t>https://million-wallpapers.ru//wallpapers/5/82/456004843638851/buket-nezhnyx-rozovyx-roz.jpg https://million-wallpapers.ru//wallpapers/4/79/13477515223342528157/buket-iz-allyx-roz-vmvaze.jpg</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">
@@ -765,7 +765,7 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>26/04/2025 01:40</t>
+          <t>27/04/2025 20:29</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
@@ -790,7 +790,7 @@
 Так же наши флористы могут собрать букет любой сложности, в любом
 оформлении - просто сообщите о своих пожеланиях при заказе менеджеру, и МЫ
 СДЕЛАЕМ КРАСИВО!
-Артикул позиции - ARTICLE764266
+Артикул позиции - ARTICLE360331
 Возможно, Вы искали: свежие цветы оптом, свежие тюльпаны, желтые, красные,
 розовые, фиолетовые
 ☎️</t>
@@ -803,7 +803,7 @@
       </c>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>https://million-wallpapers.ru/wallpapers/4/79/13477515223342528157/buket-iz-allyx-roz-vmvaze.jpg https://million-wallpapers.ru/wallpapers/5/8/14247202590552932309/krasivyj-buket-cvetov-iz-zheltyx-i-rozovyx-roz-v-upakovke.jpg https://million-wallpapers.ru/wallpapers/4/55/18073087252273351224/buket-krasivyx-roz-v-vaze.jpg</t>
+          <t>https://million-wallpapers.ru//wallpapers/4/79/13477515223342528157/buket-iz-allyx-roz-vmvaze.jpg https://million-wallpapers.ru//wallpapers/5/8/14247202590552932309/krasivyj-buket-cvetov-iz-zheltyx-i-rozovyx-roz-v-upakovke.jpg</t>
         </is>
       </c>
       <c r="G6" s="1" t="inlineStr">
@@ -835,7 +835,7 @@
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>26/04/2025 01:40</t>
+          <t>27/04/2025 20:29</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
@@ -860,7 +860,7 @@
 Так же наши флористы могут собрать букет любой сложности, в любом
 оформлении - просто сообщите о своих пожеланиях при заказе менеджеру, и МЫ
 СДЕЛАЕМ КРАСИВО!
-Артикул позиции - ARTICLE337979
+Артикул позиции - ARTICLE248588
 Возможно, Вы искали: свежие цветы оптом, свежие тюльпаны, желтые, красные,
 розовые, фиолетовые
 ☎️</t>
@@ -873,7 +873,7 @@
       </c>
       <c r="F7" s="1" t="inlineStr">
         <is>
-          <t>https://million-wallpapers.ru/wallpapers/1/53/512925356331958/cvety-tyulpany-v-bukete-na-prirode.jpg https://million-wallpapers.ru/wallpapers/6/48/548266671744531/belye-i-zholtye-tyulpany-v-bukete.jpg https://million-wallpapers.ru/wallpapers/3/16/17254999405970905524/buket-tyulpanov-k-zhenskomu-prazdniku.jpg</t>
+          <t>https://million-wallpapers.ru//wallpapers/1/53/512925356331958/cvety-tyulpany-v-bukete-na-prirode.jpg https://million-wallpapers.ru//wallpapers/6/48/548266671744531/belye-i-zholtye-tyulpany-v-bukete.jpg</t>
         </is>
       </c>
       <c r="G7" s="1" t="inlineStr">
@@ -905,7 +905,7 @@
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>26/04/2025 01:40</t>
+          <t>27/04/2025 20:29</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
@@ -930,7 +930,7 @@
 Так же наши флористы могут собрать букет любой сложности, в любом
 оформлении - просто сообщите о своих пожеланиях при заказе менеджеру, и МЫ
 СДЕЛАЕМ КРАСИВО!
-Артикул позиции - ARTICLE887164
+Артикул позиции - ARTICLE349967
 Возможно, Вы искали: свежие цветы оптом, свежие тюльпаны, желтые, красные,
 розовые, фиолетовые
 ☎️</t>
@@ -943,7 +943,7 @@
       </c>
       <c r="F8" s="1" t="inlineStr">
         <is>
-          <t>https://million-wallpapers.ru/wallpapers/1/67/433593986611635/krasnye-cvety-tyulpany-na-chernom-fone.jpg https://million-wallpapers.ru/wallpapers/1/53/512925356331958/cvety-tyulpany-v-bukete-na-prirode.jpg https://million-wallpapers.ru/wallpapers/4/43/10339545299815852394/kak-prekrasny-cvety-tyulpany-v-sadu.jpg</t>
+          <t>https://million-wallpapers.ru//wallpapers/1/67/433593986611635/krasnye-cvety-tyulpany-na-chernom-fone.jpg https://million-wallpapers.ru//wallpapers/1/53/512925356331958/cvety-tyulpany-v-bukete-na-prirode.jpg</t>
         </is>
       </c>
       <c r="G8" s="1" t="inlineStr">
@@ -975,7 +975,7 @@
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>26/04/2025 01:40</t>
+          <t>27/04/2025 20:29</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr">
@@ -1000,7 +1000,7 @@
 Так же наши флористы могут собрать букет любой сложности, в любом
 оформлении - просто сообщите о своих пожеланиях при заказе менеджеру, и МЫ
 СДЕЛАЕМ КРАСИВО!
-Артикул позиции - ARTICLE893854
+Артикул позиции - ARTICLE119722
 Возможно, Вы искали: свежие цветы оптом, свежие тюльпаны, желтые, красные,
 розовые, фиолетовые
 ☎️</t>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="F9" s="1" t="inlineStr">
         <is>
-          <t>https://million-wallpapers.ru/wallpapers/3/68/17903109010812087200/buket-tyulpanov-vesna-svezhie-cvety.jpg https://million-wallpapers.ru/wallpapers/3/25/15932062947058936005/tyulpany-park-derevya-priroda.jpg https://million-wallpapers.ru/wallpapers/1/67/433593986611635/krasnye-cvety-tyulpany-na-chernom-fone.jpg</t>
+          <t>https://million-wallpapers.ru//wallpapers/3/68/17903109010812087200/buket-tyulpanov-vesna-svezhie-cvety.jpg https://million-wallpapers.ru//wallpapers/3/25/15932062947058936005/tyulpany-park-derevya-priroda.jpg</t>
         </is>
       </c>
       <c r="G9" s="1" t="inlineStr">
@@ -1045,7 +1045,7 @@
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>26/04/2025 01:40</t>
+          <t>27/04/2025 20:29</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr">
@@ -1070,7 +1070,7 @@
 Так же наши флористы могут собрать букет любой сложности, в любом
 оформлении - просто сообщите о своих пожеланиях при заказе менеджеру, и МЫ
 СДЕЛАЕМ КРАСИВО!
-Артикул позиции - ARTICLE379471
+Артикул позиции - ARTICLE826918
 Возможно, Вы искали: свежие цветы оптом, свежие тюльпаны, желтые, красные,
 розовые, фиолетовые
 ☎️</t>
@@ -1083,7 +1083,7 @@
       </c>
       <c r="F10" s="1" t="inlineStr">
         <is>
-          <t>https://million-wallpapers.ru/wallpapers/1/67/433593986611635/krasnye-cvety-tyulpany-na-chernom-fone.jpg https://million-wallpapers.ru/wallpapers/1/59/498819012756890/oranzhevye-tyulpany-v-vedre-u-derevyannogo-fona.jpg https://million-wallpapers.ru/wallpapers/3/25/15932062947058936005/tyulpany-park-derevya-priroda.jpg</t>
+          <t>https://million-wallpapers.ru//wallpapers/1/67/433593986611635/krasnye-cvety-tyulpany-na-chernom-fone.jpg https://million-wallpapers.ru//wallpapers/1/59/498819012756890/oranzhevye-tyulpany-v-vedre-u-derevyannogo-fona.jpg</t>
         </is>
       </c>
       <c r="G10" s="1" t="inlineStr">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>26/04/2025 01:40</t>
+          <t>27/04/2025 20:29</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr">
@@ -1140,7 +1140,7 @@
 Так же наши флористы могут собрать букет любой сложности, в любом
 оформлении - просто сообщите о своих пожеланиях при заказе менеджеру, и МЫ
 СДЕЛАЕМ КРАСИВО!
-Артикул позиции - ARTICLE599724
+Артикул позиции - ARTICLE608868
 Возможно, Вы искали: свежие цветы оптом, свежие тюльпаны, желтые, красные,
 розовые, фиолетовые
 ☎️</t>
@@ -1153,7 +1153,7 @@
       </c>
       <c r="F11" s="1" t="inlineStr">
         <is>
-          <t>https://million-wallpapers.ru/wallpapers/3/43/10318155555199159092/tri-tyulpana-raznogo-cveta.jpg https://million-wallpapers.ru/wallpapers/3/78/15551530758678137065/blednorozovye-tyulpany-priroda-cvety-pasxa.jpg https://million-wallpapers.ru/wallpapers/5/81/483654671780697/rozovye-tyulpany-pole-cvetov-na-zakate.jpg</t>
+          <t>https://million-wallpapers.ru//wallpapers/3/43/10318155555199159092/tri-tyulpana-raznogo-cveta.jpg https://million-wallpapers.ru//wallpapers/3/78/15551530758678137065/blednorozovye-tyulpany-priroda-cvety-pasxa.jpg</t>
         </is>
       </c>
       <c r="G11" s="1" t="inlineStr">

</xml_diff>